<commit_message>
Committing the changes of data driven framework -Added TC row countLogic
</commit_message>
<xml_diff>
--- a/DatadrivenFramework/src/test/java/testData/TestData.xlsx
+++ b/DatadrivenFramework/src/test/java/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B68C0F-3F6E-49F2-A7B9-F1072F6BFDC1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59471EA6-2C4B-4D56-B934-DF4B5A712844}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Apache_POI_TC</t>
   </si>
@@ -43,15 +43,29 @@
     <t>klsrcm</t>
   </si>
   <si>
-    <t>Pass</t>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Test User</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Mozilla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,7 +82,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -91,13 +105,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,19 +405,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.26953125" collapsed="true"/>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -400,11 +429,20 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +452,14 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>